<commit_message>
induction folder and single variable files
</commit_message>
<xml_diff>
--- a/variable_key.xlsx
+++ b/variable_key.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A95B7C-B3A5-480B-BF77-B23318BF0ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E3B6B5-B424-407E-970C-510E57D521C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
-    <sheet name="BOM" sheetId="3" r:id="rId2"/>
-    <sheet name="DWER" sheetId="2" r:id="rId3"/>
+    <sheet name="DOT" sheetId="4" r:id="rId2"/>
+    <sheet name="BOM" sheetId="3" r:id="rId3"/>
+    <sheet name="DWER" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="523">
   <si>
     <t>Units</t>
   </si>
@@ -1172,9 +1173,6 @@
     <t>Wind Direction</t>
   </si>
   <si>
-    <t>(ø)</t>
-  </si>
-  <si>
     <t>Wind Speed</t>
   </si>
   <si>
@@ -1367,9 +1365,6 @@
     <t>Cloud height (of first group) in feet</t>
   </si>
   <si>
-    <t>Cloud amount(of second group) in eighths</t>
-  </si>
-  <si>
     <t>Cloud height (of second group) in feet</t>
   </si>
   <si>
@@ -1530,13 +1525,94 @@
   </si>
   <si>
     <t>Bottom Depth</t>
+  </si>
+  <si>
+    <t>var00180</t>
+  </si>
+  <si>
+    <t>Tidal Height</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Cloud amount of first group in eighths</t>
+  </si>
+  <si>
+    <t>Cloud amount of third group in eighths</t>
+  </si>
+  <si>
+    <t>Cloud amount of fourth group in eighths</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud amount of first group</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud amount of second group</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud amount of third group</t>
+  </si>
+  <si>
+    <t>hPa</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>oktas</t>
+  </si>
+  <si>
+    <t>ø</t>
+  </si>
+  <si>
+    <t>Horizontal visibility</t>
+  </si>
+  <si>
+    <t>AWS visibility</t>
+  </si>
+  <si>
+    <t>Mean sea level pressure</t>
+  </si>
+  <si>
+    <t>Station level pressure</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud height of third group</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud height of second group</t>
+  </si>
+  <si>
+    <t>Ceilometer cloud height of first group</t>
+  </si>
+  <si>
+    <t>Cloud height of fourth group</t>
+  </si>
+  <si>
+    <t>Cloud height of third group</t>
+  </si>
+  <si>
+    <t>Cloud height of second group</t>
+  </si>
+  <si>
+    <t>Cloud height of first group</t>
+  </si>
+  <si>
+    <t>Cloud amount (of second group) in eighths</t>
+  </si>
+  <si>
+    <t>Cloud amount of second group in eighths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1567,6 +1643,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202122"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1633,7 +1715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1662,6 +1744,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1976,11 +2059,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407D1833-63F5-4230-AD16-32E9E48F56BB}">
-  <dimension ref="A1:D180"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A180" sqref="A180"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3563,60 +3646,60 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>377</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>378</v>
+        <v>509</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B131" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C131" s="4" t="s">
         <v>379</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>109</v>
@@ -3624,57 +3707,57 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B135" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B136" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>7</v>
@@ -3682,24 +3765,24 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>14</v>
@@ -3707,62 +3790,62 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>14</v>
@@ -3770,10 +3853,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>14</v>
@@ -3781,10 +3864,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>14</v>
@@ -3792,10 +3875,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>14</v>
@@ -3803,10 +3886,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>14</v>
@@ -3814,10 +3897,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>14</v>
@@ -3825,10 +3908,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>14</v>
@@ -3836,10 +3919,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>12</v>
@@ -3847,10 +3930,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>12</v>
@@ -3858,10 +3941,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>12</v>
@@ -3869,10 +3952,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>109</v>
@@ -3880,198 +3963,266 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>441</v>
+        <v>499</v>
+      </c>
+      <c r="C159" s="10" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+      <c r="B162" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
+      <c r="B163" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
+      <c r="B164" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
+      <c r="B165" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C165" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
+      <c r="B166" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
+      <c r="B167" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C167" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="1" t="s">
+      <c r="B168" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+      <c r="B169" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="B168" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="1" t="s">
+      <c r="B170" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B169" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="1" t="s">
+      <c r="B171" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C171" s="10" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B170" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
+      <c r="B172" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B173" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B172" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
+      <c r="B174" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
+      <c r="B175" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B176" s="1" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>459</v>
+        <v>512</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>460</v>
+        <v>513</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4082,11 +4233,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B891FCC8-6932-42EA-B0A0-1A3A06F7421B}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="2">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>VLOOKUP(C2,Key!$A$2:$B942,2,TRUE)</f>
+        <v>Tidal Height</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618D0C58-8C8E-440E-A497-ABAD71259CF4}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4109,18 +4311,19 @@
         <v>376</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B2" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>VLOOKUP(C2,Key!$A$2:$B942,2,TRUE)</f>
@@ -4129,13 +4332,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>VLOOKUP(C3,Key!$A$2:$B944,2,TRUE)</f>
@@ -4144,13 +4347,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>VLOOKUP(C4,Key!$A$2:$B946,2,TRUE)</f>
@@ -4159,13 +4362,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>VLOOKUP(C5,Key!$A$2:$B948,2,TRUE)</f>
@@ -4174,13 +4377,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>VLOOKUP(C6,Key!$A$2:$B950,2,TRUE)</f>
@@ -4189,14 +4392,14 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B7" s="1">
         <f>1/3.6</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>VLOOKUP(C7,Key!$A$2:$B952,2,TRUE)</f>
@@ -4205,13 +4408,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>VLOOKUP(C8,Key!$A$2:$B954,2,TRUE)</f>
@@ -4220,14 +4423,14 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B9" s="1">
         <f>1/3.6</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>VLOOKUP(C9,Key!$A$2:$B956,2,TRUE)</f>
@@ -4236,223 +4439,223 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>VLOOKUP(C10,Key!$A$2:$B958,2,TRUE)</f>
-        <v>Cloud amount (of first group) in eighths</v>
+        <v>Cloud amount of first group in eighths</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>VLOOKUP(C11,Key!$A$2:$B960,2,TRUE)</f>
-        <v>Cloud height (of first group) in feet</v>
+        <v>Cloud height of first group</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>443</v>
+        <v>521</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>VLOOKUP(C12,Key!$A$2:$B962,2,TRUE)</f>
-        <v>Cloud amount(of second group) in eighths</v>
+        <v>Cloud amount of second group in eighths</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>VLOOKUP(C13,Key!$A$2:$B964,2,TRUE)</f>
-        <v>Cloud height (of second group) in feet</v>
+        <v>Cloud height of second group</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>VLOOKUP(C14,Key!$A$2:$B966,2,TRUE)</f>
-        <v>Cloud amount (of third group) in eighths</v>
+        <v>Cloud amount of third group in eighths</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>VLOOKUP(C15,Key!$A$2:$B968,2,TRUE)</f>
-        <v>Cloud height (of third group) in feet</v>
+        <v>Cloud height of third group</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>VLOOKUP(C16,Key!$A$2:$B970,2,TRUE)</f>
-        <v>Cloud amount (of fourth group) in eighths</v>
+        <v>Cloud amount of fourth group in eighths</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>VLOOKUP(C17,Key!$A$2:$B972,2,TRUE)</f>
-        <v>Cloud height (of fourth group) in feet</v>
+        <v>Cloud height of fourth group</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>VLOOKUP(C18,Key!$A$2:$B974,2,TRUE)</f>
-        <v>Ceilometer cloud amount (of first group)</v>
+        <v>Ceilometer cloud amount of first group</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D19" s="2" t="str">
         <f>VLOOKUP(C19,Key!$A$2:$B976,2,TRUE)</f>
-        <v>Ceilometer cloud height (of first group) in feet</v>
+        <v>Ceilometer cloud height of first group</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>VLOOKUP(C20,Key!$A$2:$B978,2,TRUE)</f>
-        <v>Ceilometer cloud amount (of second group)</v>
+        <v>Ceilometer cloud amount of second group</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>VLOOKUP(C21,Key!$A$2:$B980,2,TRUE)</f>
-        <v>Ceilometer cloud height (of second group) in feet</v>
+        <v>Ceilometer cloud height of second group</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>VLOOKUP(C22,Key!$A$2:$B982,2,TRUE)</f>
-        <v>Ceilometer cloud amount (of third group)</v>
+        <v>Ceilometer cloud amount of third group</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D23" s="2" t="str">
         <f>VLOOKUP(C23,Key!$A$2:$B984,2,TRUE)</f>
-        <v>Ceilometer cloud height (of third group) in feet</v>
+        <v>Ceilometer cloud height of third group</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>VLOOKUP(C24,Key!$A$2:$B986,2,TRUE)</f>
@@ -4461,43 +4664,43 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>VLOOKUP(C25,Key!$A$2:$B987,2,TRUE)</f>
-        <v>Horizontal visibility in km</v>
+        <v>Horizontal visibility</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>VLOOKUP(C26,Key!$A$2:$B989,2,TRUE)</f>
-        <v>AWS visibility in km</v>
+        <v>AWS visibility</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>VLOOKUP(C27,Key!$A$2:$B991,2,TRUE)</f>
@@ -4506,32 +4709,32 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>VLOOKUP(C28,Key!$A$2:$B993,2,TRUE)</f>
-        <v>Mean sea level pressure in hPa</v>
+        <v>Mean sea level pressure</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D29" s="2" t="str">
         <f>VLOOKUP(C29,Key!$A$2:$B995,2,TRUE)</f>
-        <v>Station level pressure in hPa</v>
+        <v>Station level pressure</v>
       </c>
     </row>
   </sheetData>
@@ -4540,12 +4743,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F53C71-6126-496F-BF12-2421C1B2ABC6}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4567,7 +4770,7 @@
         <v>376</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4578,7 +4781,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>VLOOKUP(C2,Key!$A$2:$B942,2,TRUE)</f>
@@ -4593,7 +4796,7 @@
         <v>-1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>VLOOKUP(C3,Key!$A$2:$B943,2,TRUE)</f>
@@ -4620,8 +4823,7 @@
         <v>337</v>
       </c>
       <c r="B5" s="2">
-        <f>1/1000</f>
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>219</v>
@@ -4636,11 +4838,10 @@
         <v>338</v>
       </c>
       <c r="B6" s="2">
-        <f>1/1000</f>
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>VLOOKUP(C6,Key!$A$2:$B946,2,TRUE)</f>
@@ -4652,11 +4853,10 @@
         <v>339</v>
       </c>
       <c r="B7" s="2">
-        <f>1/1000</f>
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>VLOOKUP(C7,Key!$A$2:$B947,2,TRUE)</f>
@@ -4671,7 +4871,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>VLOOKUP(C8,Key!$A$2:$B948,2,TRUE)</f>
@@ -4686,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>VLOOKUP(C9,Key!$A$2:$B949,2,TRUE)</f>
@@ -4701,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>VLOOKUP(C10,Key!$A$2:$B950,2,TRUE)</f>
@@ -4716,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>VLOOKUP(C11,Key!$A$2:$B951,2,TRUE)</f>
@@ -4728,7 +4928,8 @@
         <v>344</v>
       </c>
       <c r="B12" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>237</v>
@@ -4743,7 +4944,8 @@
         <v>345</v>
       </c>
       <c r="B13" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>231</v>
@@ -4758,10 +4960,11 @@
         <v>346</v>
       </c>
       <c r="B14" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D14" s="2" t="str">
         <f>VLOOKUP(C14,Key!$A$2:$B954,2,TRUE)</f>
@@ -4773,7 +4976,8 @@
         <v>347</v>
       </c>
       <c r="B15" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>214</v>
@@ -4788,7 +4992,8 @@
         <v>348</v>
       </c>
       <c r="B16" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>230</v>
@@ -4833,7 +5038,8 @@
         <v>351</v>
       </c>
       <c r="B19" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>215</v>
@@ -4851,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>VLOOKUP(C20,Key!$A$2:$B960,2,TRUE)</f>
@@ -4866,7 +5072,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>VLOOKUP(C21,Key!$A$2:$B961,2,TRUE)</f>
@@ -4878,7 +5084,8 @@
         <v>354</v>
       </c>
       <c r="B22" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>232</v>
@@ -4911,7 +5118,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>VLOOKUP(C24,Key!$A$2:$B964,2,TRUE)</f>
@@ -4923,7 +5130,8 @@
         <v>357</v>
       </c>
       <c r="B25" s="2">
-        <v>1000</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>229</v>
@@ -4971,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D28" s="2" t="str">
         <f>VLOOKUP(C28,Key!$A$2:$B968,2,TRUE)</f>
@@ -5001,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D30" s="2" t="str">
         <f>VLOOKUP(C30,Key!$A$2:$B970,2,TRUE)</f>
@@ -5017,7 +5225,7 @@
         <v>0.51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>VLOOKUP(C31,Key!$A$2:$B971,2,TRUE)</f>
@@ -5032,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D32" s="2" t="str">
         <f>VLOOKUP(C32,Key!$A$2:$B972,2,TRUE)</f>
@@ -5047,7 +5255,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D33" s="2" t="str">
         <f>VLOOKUP(C33,Key!$A$2:$B973,2,TRUE)</f>
@@ -5062,7 +5270,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D34" s="2" t="str">
         <f>VLOOKUP(C34,Key!$A$2:$B974,2,TRUE)</f>
@@ -5077,7 +5285,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D35" s="2" t="str">
         <f>VLOOKUP(C35,Key!$A$2:$B975,2,TRUE)</f>
@@ -5092,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D36" s="2" t="str">
         <f>VLOOKUP(C36,Key!$A$2:$B976,2,TRUE)</f>
@@ -5107,7 +5315,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>VLOOKUP(C37,Key!$A$2:$B977,2,TRUE)</f>
@@ -5122,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D38" s="2" t="str">
         <f>VLOOKUP(C38,Key!$A$2:$B978,2,TRUE)</f>
@@ -5137,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D39" s="2" t="str">
         <f>VLOOKUP(C39,Key!$A$2:$B979,2,TRUE)</f>
@@ -5152,7 +5360,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D40" s="2" t="str">
         <f>VLOOKUP(C40,Key!$A$2:$B980,2,TRUE)</f>
@@ -5167,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D41" s="2" t="str">
         <f>VLOOKUP(C41,Key!$A$2:$B981,2,TRUE)</f>

</xml_diff>

<commit_message>
Updated headers with new attributes
</commit_message>
<xml_diff>
--- a/variable_key.xlsx
+++ b/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E3B6B5-B424-407E-970C-510E57D521C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DC4C81-3845-455D-88C5-8A56E1558305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -1515,9 +1515,6 @@
     <t>Max Wind Speed</t>
   </si>
   <si>
-    <t>(mL)</t>
-  </si>
-  <si>
     <t>Chlorophyll sample volume</t>
   </si>
   <si>
@@ -1606,6 +1603,9 @@
   </si>
   <si>
     <t>Cloud amount of second group in eighths</t>
+  </si>
+  <si>
+    <t>mL</t>
   </si>
 </sst>
 </file>
@@ -2062,20 +2062,20 @@
   <dimension ref="A1:D181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B161" sqref="B161"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>206</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>207</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>208</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>209</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>210</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>211</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>212</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>213</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>214</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>215</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>216</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>217</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>218</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>219</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>220</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>221</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>222</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>223</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>224</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>225</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>226</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>227</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>228</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>229</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>230</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>231</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>232</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>233</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>234</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>235</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>236</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>237</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>238</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>239</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>240</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>242</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>243</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>244</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>245</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>246</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>247</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>248</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>249</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>250</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>251</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>252</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>253</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>254</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>255</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>256</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>257</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>258</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>259</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>260</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>261</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>262</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>263</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>264</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>265</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>266</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>267</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>268</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>269</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>270</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>271</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>272</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>273</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>274</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>275</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>276</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>277</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>278</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>279</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>280</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>281</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>282</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>283</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>284</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>285</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>286</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>287</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>288</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>289</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>290</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>291</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>292</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>293</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>294</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>295</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>296</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>297</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>298</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>299</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>300</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>301</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>302</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>303</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>304</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>305</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>306</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>307</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>308</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>309</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>310</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>311</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>312</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>313</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>314</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>315</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>316</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>318</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>319</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>320</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>321</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>322</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>323</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>324</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>325</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>326</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>327</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>328</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>329</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>330</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>331</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>332</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>333</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>380</v>
       </c>
@@ -3652,10 +3652,10 @@
         <v>377</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>381</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>386</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>387</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>389</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>392</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>395</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>397</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>401</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>403</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>406</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>408</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>410</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>422</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>423</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>424</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>425</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>426</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>427</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>428</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>429</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>430</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>431</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>460</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>461</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>462</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>463</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>464</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>465</v>
       </c>
@@ -3972,161 +3972,161 @@
         <v>379</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>466</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>467</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>468</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>469</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>470</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>471</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>472</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>473</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>474</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>475</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>476</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>477</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>478</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>480</v>
       </c>
@@ -4134,29 +4134,29 @@
         <v>453</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>481</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>482</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>483</v>
       </c>
@@ -4164,45 +4164,45 @@
         <v>456</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>484</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>485</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>486</v>
       </c>
       <c r="B179" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="C179" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
+      <c r="B180" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>495</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>14</v>
@@ -4211,12 +4211,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>497</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>14</v>
@@ -4240,14 +4240,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>374</v>
       </c>
@@ -4261,16 +4261,16 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B2" s="2">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>VLOOKUP(C2,Key!$A$2:$B942,2,TRUE)</f>
@@ -4291,16 +4291,16 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>374</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>432</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>Precipitation</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>433</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>Air Temperature</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>434</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>Wet Bulb Air Temperature</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>435</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>Dew Point Temperature</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>436</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>Relative Humidity</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>437</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>Wind Speed</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>438</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>Wind Direction</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>439</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>Max Wind Speed</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>440</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>Cloud amount of first group in eighths</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>441</v>
       </c>
@@ -4467,9 +4467,9 @@
         <v>Cloud height of first group</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -4482,7 +4482,7 @@
         <v>Cloud amount of second group in eighths</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>442</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>Cloud height of second group</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>443</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>Cloud amount of third group in eighths</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>444</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>Cloud height of third group</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>445</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>Cloud amount of fourth group in eighths</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>446</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>Cloud height of fourth group</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>447</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>Ceilometer cloud amount of first group</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>448</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>Ceilometer cloud height of first group</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>449</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>Ceilometer cloud amount of second group</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>450</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>Ceilometer cloud height of second group</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>451</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>Ceilometer cloud amount of third group</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>452</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>Ceilometer cloud height of third group</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>453</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>Ceilometer sky clear flag</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>454</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>Horizontal visibility</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>455</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>AWS visibility</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>456</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>Present weather in code</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>457</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>Mean sea level pressure</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>458</v>
       </c>
@@ -4751,15 +4751,15 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" style="2"/>
-    <col min="4" max="4" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="36.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>374</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>334</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>Total Alkalinity</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>335</v>
       </c>
@@ -4796,14 +4796,14 @@
         <v>-1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>VLOOKUP(C3,Key!$A$2:$B943,2,TRUE)</f>
         <v>Bottom Depth</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>336</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>Dissolved Organic Carbon</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>337</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>Chlorophyll-a</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>338</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>Chlorophyll-b</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>339</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>Chlorophyll-c</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>340</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>Chlorophyll sample volume</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>341</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>Cloud Cover</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>342</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>Conductivity</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>343</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>Flow Status</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>344</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>Dissolved Organic Nitrogen</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>345</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>Nitrate</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>346</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>Total TKN</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>347</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>Total Nitrogen</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>348</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>Ammonium</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>349</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>O2 Saturation</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>350</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>Oxygen</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>351</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>Total Phosphorus</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>352</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>pH</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>353</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>Phaeophytin a</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>354</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>Filterable Reactive Phosphate</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>355</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>Salinity</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>356</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>Secchi depth</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>357</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>Reactive Silica</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>358</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>Total Suspended Solids</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>359</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>Temperature</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>360</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>Tide status</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>361</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>Turbidity</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>362</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>Wind Direction</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>363</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>Wind Speed</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>364</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>Max Discharge</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>365</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>Mean Discharge</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>366</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>Min Discharge</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>367</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>Discharge</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>368</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>Max Stage Height CTF</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>369</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>Mean Stage Height CTF</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>370</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>Min Stage Height CTF</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>371</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>Max Stage Height</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>372</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>Mean Stage Height</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>373</v>
       </c>

</xml_diff>